<commit_message>
Added and adapted Yarpiz PSO implementation. Added run_pso and PSO class
</commit_message>
<xml_diff>
--- a/tables/DE/DE_best_1_bin_F_09_Cr_09_pop_30/DE_table2_F14_dim10.xlsx
+++ b/tables/DE/DE_best_1_bin_F_09_Cr_09_pop_30/DE_table2_F14_dim10.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
-  <si>
-    <t>Gen</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
+  <si>
+    <t>MaxFES</t>
   </si>
   <si>
     <t>Run  0</t>
@@ -167,9 +167,6 @@
   </si>
   <si>
     <t>Run 49</t>
-  </si>
-  <si>
-    <t>Run 50</t>
   </si>
   <si>
     <t>Mean</t>
@@ -526,7 +523,7 @@
     <s:outlinePr summaryBelow="1" summaryRight="1"/>
     <s:pageSetUpPr/>
   </s:sheetPr>
-  <dimension ref="A1:BA14"/>
+  <dimension ref="A1:AZ14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -534,7 +531,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:53">
+    <row r="1" spans="1:52">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -691,11 +688,8 @@
       <c r="AZ1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="1" t="s">
-        <v>52</v>
-      </c>
     </row>
-    <row r="2" spans="1:53">
+    <row r="2" spans="1:52">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
@@ -850,15 +844,12 @@
         <v>101.93040546</v>
       </c>
       <c r="AZ2" t="n">
-        <v>78.28139349</v>
-      </c>
-      <c r="BA2" t="n">
-        <v>66.03883613000001</v>
+        <v>65.79398498</v>
       </c>
     </row>
-    <row r="3" spans="1:53">
+    <row r="3" spans="1:52">
       <c r="A3" s="1" t="n">
-        <v>3</v>
+        <v>0.001</v>
       </c>
       <c r="B3" t="n">
         <v>19.35863676</v>
@@ -1011,15 +1002,12 @@
         <v>57.16310005</v>
       </c>
       <c r="AZ3" t="n">
-        <v>56.00086452</v>
-      </c>
-      <c r="BA3" t="n">
-        <v>49.71789629</v>
+        <v>49.59223693</v>
       </c>
     </row>
-    <row r="4" spans="1:53">
+    <row r="4" spans="1:52">
       <c r="A4" s="1" t="n">
-        <v>33</v>
+        <v>0.01</v>
       </c>
       <c r="B4" t="n">
         <v>2.80847539</v>
@@ -1172,15 +1160,12 @@
         <v>0.50379286</v>
       </c>
       <c r="AZ4" t="n">
-        <v>3.06622269</v>
-      </c>
-      <c r="BA4" t="n">
-        <v>3.00443004</v>
+        <v>3.00319419</v>
       </c>
     </row>
-    <row r="5" spans="1:53">
+    <row r="5" spans="1:52">
       <c r="A5" s="1" t="n">
-        <v>333</v>
+        <v>0.1</v>
       </c>
       <c r="B5" t="n">
         <v>0.20174215</v>
@@ -1333,15 +1318,12 @@
         <v>0.20238698</v>
       </c>
       <c r="AZ5" t="n">
-        <v>0.21064809</v>
-      </c>
-      <c r="BA5" t="n">
-        <v>0.2393568</v>
+        <v>0.23993097</v>
       </c>
     </row>
-    <row r="6" spans="1:53">
+    <row r="6" spans="1:52">
       <c r="A6" s="1" t="n">
-        <v>666</v>
+        <v>0.2</v>
       </c>
       <c r="B6" t="n">
         <v>0.1549291</v>
@@ -1494,15 +1476,12 @@
         <v>0.20238698</v>
       </c>
       <c r="AZ6" t="n">
-        <v>0.15622104</v>
-      </c>
-      <c r="BA6" t="n">
-        <v>0.20621734</v>
+        <v>0.20721726</v>
       </c>
     </row>
-    <row r="7" spans="1:53">
+    <row r="7" spans="1:52">
       <c r="A7" s="1" t="n">
-        <v>1000</v>
+        <v>0.3</v>
       </c>
       <c r="B7" t="n">
         <v>0.12808883</v>
@@ -1655,15 +1634,12 @@
         <v>0.20238698</v>
       </c>
       <c r="AZ7" t="n">
-        <v>0.15622104</v>
-      </c>
-      <c r="BA7" t="n">
-        <v>0.18421314</v>
+        <v>0.18477299</v>
       </c>
     </row>
-    <row r="8" spans="1:53">
+    <row r="8" spans="1:52">
       <c r="A8" s="1" t="n">
-        <v>1333</v>
+        <v>0.4</v>
       </c>
       <c r="B8" t="n">
         <v>0.12808883</v>
@@ -1816,15 +1792,12 @@
         <v>0.20238698</v>
       </c>
       <c r="AZ8" t="n">
-        <v>0.15622104</v>
-      </c>
-      <c r="BA8" t="n">
-        <v>0.17039904</v>
+        <v>0.1706826</v>
       </c>
     </row>
-    <row r="9" spans="1:53">
+    <row r="9" spans="1:52">
       <c r="A9" s="1" t="n">
-        <v>1666</v>
+        <v>0.5</v>
       </c>
       <c r="B9" t="n">
         <v>0.12808883</v>
@@ -1977,15 +1950,12 @@
         <v>0.16131304</v>
       </c>
       <c r="AZ9" t="n">
-        <v>0.11803774</v>
-      </c>
-      <c r="BA9" t="n">
-        <v>0.15434272</v>
+        <v>0.15506882</v>
       </c>
     </row>
-    <row r="10" spans="1:53">
+    <row r="10" spans="1:52">
       <c r="A10" s="1" t="n">
-        <v>1999</v>
+        <v>0.6</v>
       </c>
       <c r="B10" t="n">
         <v>0.12808883</v>
@@ -2138,15 +2108,12 @@
         <v>0.16131304</v>
       </c>
       <c r="AZ10" t="n">
-        <v>0.11803774</v>
-      </c>
-      <c r="BA10" t="n">
-        <v>0.14626902</v>
+        <v>0.14683365</v>
       </c>
     </row>
-    <row r="11" spans="1:53">
+    <row r="11" spans="1:52">
       <c r="A11" s="1" t="n">
-        <v>2332</v>
+        <v>0.7</v>
       </c>
       <c r="B11" t="n">
         <v>0.12808883</v>
@@ -2299,15 +2266,12 @@
         <v>0.14991233</v>
       </c>
       <c r="AZ11" t="n">
-        <v>0.11803774</v>
-      </c>
-      <c r="BA11" t="n">
-        <v>0.14075223</v>
+        <v>0.14120652</v>
       </c>
     </row>
-    <row r="12" spans="1:53">
+    <row r="12" spans="1:52">
       <c r="A12" s="1" t="n">
-        <v>2666</v>
+        <v>0.8</v>
       </c>
       <c r="B12" t="n">
         <v>0.11831345</v>
@@ -2460,15 +2424,12 @@
         <v>0.14991233</v>
       </c>
       <c r="AZ12" t="n">
-        <v>0.11803774</v>
-      </c>
-      <c r="BA12" t="n">
-        <v>0.13230134</v>
+        <v>0.13258661</v>
       </c>
     </row>
-    <row r="13" spans="1:53">
+    <row r="13" spans="1:52">
       <c r="A13" s="1" t="n">
-        <v>2999</v>
+        <v>0.9</v>
       </c>
       <c r="B13" t="n">
         <v>0.11831345</v>
@@ -2621,15 +2582,12 @@
         <v>0.14991233</v>
       </c>
       <c r="AZ13" t="n">
-        <v>0.10355863</v>
-      </c>
-      <c r="BA13" t="n">
-        <v>0.12692025</v>
+        <v>0.12738748</v>
       </c>
     </row>
-    <row r="14" spans="1:53">
+    <row r="14" spans="1:52">
       <c r="A14" s="1" t="n">
-        <v>3332</v>
+        <v>1</v>
       </c>
       <c r="B14" t="n">
         <v>0.11831345</v>
@@ -2782,10 +2740,7 @@
         <v>0.13947101</v>
       </c>
       <c r="AZ14" t="n">
-        <v>0.10355863</v>
-      </c>
-      <c r="BA14" t="n">
-        <v>0.12488043</v>
+        <v>0.12530687</v>
       </c>
     </row>
   </sheetData>

</xml_diff>